<commit_message>
added yield modifier, animal product adjust to western diet
1. Changed Brazil responsiveness input in spreadsheet so that it runs from 2001-2030.
2. Added yield modifier for Maize, OilCrop, for US and EU.  Specify as year-by-year percentage deviation from baseline. 0 means run baseline scenario. -25 means 25% reduction in yield; 20 means 20% increase in yield.
3. Set mechanism to adjust animal product per-capita demand in China to get closer to western demand. Defined as first-order exponential (half-way to wall) process. Set switch to 1 to activate. Set start time and exponential averaging time also.
4. set stop time for simulation to 2030.

YET TO DO: Push output metrics into spreadsheet.
</commit_message>
<xml_diff>
--- a/Models/BioLUC-CRAFTY-2000/Data/BrazilResponsiveness.xlsx
+++ b/Models/BioLUC-CRAFTY-2000/Data/BrazilResponsiveness.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\GitHub\CRAFTY-BioLuc\Models\BioLUC-CRAFTY-2000\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69883FCE-4F19-4576-A241-E052AF3B17B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0327E1C4-E7A0-4F80-AEAF-3C4DD55CF324}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27465" yWindow="465" windowWidth="26520" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Global.BRA_Maize_Responsiveness</t>
   </si>
@@ -34,6 +34,27 @@
   </si>
   <si>
     <t>Global.BRA_Beef_Responsiveness</t>
+  </si>
+  <si>
+    <t>USA.C_yield_variation_PCT[Maize]</t>
+  </si>
+  <si>
+    <t>USA.C_yield_variation_PCT[OilCrop]</t>
+  </si>
+  <si>
+    <t>EU27.C_yield_variation_PCT[Maize]</t>
+  </si>
+  <si>
+    <t>EU27.C_yield_variation_PCT[OilCrop]</t>
+  </si>
+  <si>
+    <t>CHIHKG.TransitionToWesternDiet</t>
+  </si>
+  <si>
+    <t>CHIHKG.DietTransition Start</t>
+  </si>
+  <si>
+    <t>CHIHKG.DietTransitionTime</t>
   </si>
 </sst>
 </file>
@@ -365,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,7 +397,7 @@
     <col min="1" max="1" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +464,35 @@
       <c r="V1" s="1">
         <v>1.75</v>
       </c>
+      <c r="W1" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="X1" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>1.75</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -511,8 +559,35 @@
       <c r="V3">
         <v>0.60899999999999999</v>
       </c>
+      <c r="W3">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="X3">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="Y3">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="Z3">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="AA3">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="AB3">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="AC3">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="AD3">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="AE3">
+        <v>0.60899999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -578,6 +653,437 @@
       </c>
       <c r="V5">
         <v>0.01</v>
+      </c>
+      <c r="W5">
+        <v>0.01</v>
+      </c>
+      <c r="X5">
+        <v>0.01</v>
+      </c>
+      <c r="Y5">
+        <v>0.01</v>
+      </c>
+      <c r="Z5">
+        <v>0.01</v>
+      </c>
+      <c r="AA5">
+        <v>0.01</v>
+      </c>
+      <c r="AB5">
+        <v>0.01</v>
+      </c>
+      <c r="AC5">
+        <v>0.01</v>
+      </c>
+      <c r="AD5">
+        <v>0.01</v>
+      </c>
+      <c r="AE5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds connection to change in meat demand for 3 regions
CHIHKG.DietTransitionTime	5

Global.AP demand mod pct[USA 1]	0

Global.AP demand mod pct[EU27 1]	0

Global.AP demand mod pct[CHIHKG 1]	0

set to negative percentage (e..g., -30) to change meat demand relative to  baseline scenario.  Phase in occurs between 2015-2020.
</commit_message>
<xml_diff>
--- a/Models/BioLUC-CRAFTY-2000/Data/BrazilResponsiveness.xlsx
+++ b/Models/BioLUC-CRAFTY-2000/Data/BrazilResponsiveness.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\GitHub\CRAFTY-BioLuc\Models\BioLUC-CRAFTY-2000\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0327E1C4-E7A0-4F80-AEAF-3C4DD55CF324}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A672C-97F0-4AF5-8B78-24879EEDD574}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30390" yWindow="960" windowWidth="26520" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Global.BRA_Maize_Responsiveness</t>
   </si>
@@ -42,12 +42,6 @@
     <t>USA.C_yield_variation_PCT[OilCrop]</t>
   </si>
   <si>
-    <t>EU27.C_yield_variation_PCT[Maize]</t>
-  </si>
-  <si>
-    <t>EU27.C_yield_variation_PCT[OilCrop]</t>
-  </si>
-  <si>
     <t>CHIHKG.TransitionToWesternDiet</t>
   </si>
   <si>
@@ -55,6 +49,21 @@
   </si>
   <si>
     <t>CHIHKG.DietTransitionTime</t>
+  </si>
+  <si>
+    <t>Global.AP demand mod pct[USA 1]</t>
+  </si>
+  <si>
+    <t>Global.AP demand mod pct[EU27 1]</t>
+  </si>
+  <si>
+    <t>Global.AP demand mod pct[CHIHKG 1]</t>
+  </si>
+  <si>
+    <t>EU 27.C_yield_variation_PCT[Maize]</t>
+  </si>
+  <si>
+    <t>EU 27.C_yield_variation_PCT[OilCrop]</t>
   </si>
 </sst>
 </file>
@@ -386,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE19"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +883,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -969,7 +978,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1064,7 +1073,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1072,7 +1081,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>2020</v>
@@ -1080,10 +1089,34 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>